<commit_message>
commit on 15th may with config reader
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/dsAlgoInput.xlsx
+++ b/src/test/resources/excel/dsAlgoInput.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AKandan1/eclipse-workspace/DsAlgoProject/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AKandan1/eclipse-workspace/dsalgoprojectframework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872724F2-7E74-DD41-8314-4CED8B32AFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1593D3F9-06EA-3941-91A1-6AD3977C3ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{E9D9CA53-B914-144C-BF20-F219DFBBDED7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>TestCaseNo</t>
   </si>
@@ -93,16 +93,69 @@
   </si>
   <si>
     <t>tag7</t>
+  </si>
+  <si>
+    <t>tag8</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Password should contain at least 8 characters</t>
+  </si>
+  <si>
+    <t>Password can’t be entirely numeric.</t>
+  </si>
+  <si>
+    <t>tag9</t>
+  </si>
+  <si>
+    <t>tag10</t>
+  </si>
+  <si>
+    <t>tag11</t>
+  </si>
+  <si>
+    <t>tag12</t>
+  </si>
+  <si>
+    <t>testsdet84</t>
+  </si>
+  <si>
+    <t>password can’t be too similar to your other personal information.</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>Password can’t be commonly used password</t>
+  </si>
+  <si>
+    <t>numpyqueen</t>
+  </si>
+  <si>
+    <t>queen@1305</t>
+  </si>
+  <si>
+    <t>New Account Created. You are logged in as numpyqueen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,13 +178,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC537017-09E8-E244-B2AF-B906A77F7185}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,7 +511,7 @@
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="71" customWidth="1"/>
+    <col min="5" max="5" width="84.83203125" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,7 +603,7 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
@@ -558,6 +614,91 @@
       </c>
       <c r="E7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>123456789</v>
+      </c>
+      <c r="D9">
+        <v>123456789</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -566,6 +707,12 @@
     <hyperlink ref="B7" r:id="rId2" xr:uid="{7DC3E653-B2F9-3849-99D7-891A842F3BED}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{5520B8BF-0187-4045-A882-7D1F4C7F164B}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{40CEC0FA-F2ED-5441-B9E1-99B575E4461E}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{6669F510-1E5B-8F4C-A680-18DB2AEBD1E6}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{B1DB5CFE-23F3-734E-9AC6-692A08A03B8D}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{B0287FEB-118C-8845-B07A-8045E68EC3A1}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{62745BC6-582E-6E4D-BBC0-E12A124CBD01}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{245A67E1-D2CE-494C-B981-3537BAF11935}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{D4FCD26B-72D1-A14C-860B-4C76DEE8B91B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit My changes 22may
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/dsAlgoInput.xlsx
+++ b/src/test/resources/excel/dsAlgoInput.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AKandan1/eclipse-workspace/dsalgoprojectframework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1593D3F9-06EA-3941-91A1-6AD3977C3ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BAFED5-0009-8D40-8321-70AC2EF6EB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{E9D9CA53-B914-144C-BF20-F219DFBBDED7}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{E9D9CA53-B914-144C-BF20-F219DFBBDED7}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterPage" sheetId="1" r:id="rId1"/>
+    <sheet name="LinkedlistPage" sheetId="2" r:id="rId2"/>
+    <sheet name="Treepage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>TestCaseNo</t>
   </si>
@@ -138,13 +140,48 @@
   </si>
   <si>
     <t>New Account Created. You are logged in as numpyqueen</t>
+  </si>
+  <si>
+    <t>Pythoncode</t>
+  </si>
+  <si>
+    <t>Runresult</t>
+  </si>
+  <si>
+    <t>testCaseNo6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num1 = 1.5
+num2 = 6.3
+sum = num1 + num2 
+print('The sum of {0} and {1} is {2}'.format(num1, num2, sum))
+</t>
+  </si>
+  <si>
+    <t>The sum of 1.5 and 6.3 is 7.8</t>
+  </si>
+  <si>
+    <t>testCaseNo7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num1 = 1.5
+num2 = 6.3
+sum = num1 + num2 
+print('The sum of {0} and {1} is {2}'.format(num1, num2, 
+</t>
+  </si>
+  <si>
+    <t>SyntaxError: EOF in multi-line statement on line 6</t>
+  </si>
+  <si>
+    <t>The sum of 1.5 and 6.3 is 7.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +193,19 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,9 +232,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -502,9 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC537017-09E8-E244-B2AF-B906A77F7185}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -718,6 +772,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311F7144-09FD-8940-8259-41CAD088AA87}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="65.5" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08141162-47B3-594C-AEB8-5A1219C8C50E}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="88" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{7af72c41-31f4-4d40-a6d0-808117dc4d77}" enabled="1" method="Standard" siteId="{be0f980b-dd99-4b19-bd7b-bc71a09b026c}" contentBits="0" removed="0"/>

</xml_diff>